<commit_message>
First set of budget test working.
</commit_message>
<xml_diff>
--- a/forecast/test/test_assets/budget_upload_bad_data.xlsx
+++ b/forecast/test/test_assets/budget_upload_bad_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stronal/PycharmProjects/fido/forecast/test/test_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9805B5D4-CF73-1D4B-AB71-2CFBCD2D74E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F78A10-DF02-5E46-9C81-42F37028E35C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -934,11 +934,12 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
@@ -1001,10 +1002,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>109010</v>
+        <v>109076</v>
       </c>
       <c r="B2">
-        <v>14112001</v>
+        <v>11272001</v>
       </c>
       <c r="C2">
         <v>310945</v>
@@ -1119,12 +1120,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1133,7 +1128,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CB92EEA46F33934A96D04653E9CD3A46" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9eaa3db9b0a4b6d7e344c4c898640736">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9a67a83b-a5e1-4318-948d-450fbb0b26a1" xmlns:ns4="e48749df-3746-4597-97ee-799f462add48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f3412b8a302904ea294823bd47e66978" ns3:_="" ns4:_="">
     <xsd:import namespace="9a67a83b-a5e1-4318-948d-450fbb0b26a1"/>
@@ -1342,24 +1337,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F34B647-70B2-425E-B00E-F8374E364F8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e48749df-3746-4597-97ee-799f462add48"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9a67a83b-a5e1-4318-948d-450fbb0b26a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADF255A-1CA2-4DE5-95FF-3D43C4BC1A95}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1367,7 +1351,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CA1EFC-4563-470C-8C14-A71BA4C05637}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1384,4 +1368,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F34B647-70B2-425E-B00E-F8374E364F8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e48749df-3746-4597-97ee-799f462add48"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9a67a83b-a5e1-4318-948d-450fbb0b26a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Feature/error during upload (#91)
Produce warning and error reports when uploading Budgets or Actuals from an Excel file.
Improve performance by reducing the numbers of read from the database and using a different way to read the Excel file.
Add heuristic message during the upload.
Lock the correct columns when downloading from the Edit Forecast page.
</commit_message>
<xml_diff>
--- a/forecast/test/test_assets/budget_upload_bad_data.xlsx
+++ b/forecast/test/test_assets/budget_upload_bad_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stronal/PycharmProjects/fido/forecast/test/test_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F78A10-DF02-5E46-9C81-42F37028E35C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9381B3F-FBA6-CC4A-80EC-6E6D3306E8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -934,7 +934,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1120,12 +1120,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1338,15 +1335,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADF255A-1CA2-4DE5-95FF-3D43C4BC1A95}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F34B647-70B2-425E-B00E-F8374E364F8C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e48749df-3746-4597-97ee-799f462add48"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9a67a83b-a5e1-4318-948d-450fbb0b26a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1371,18 +1380,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F34B647-70B2-425E-B00E-F8374E364F8C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADF255A-1CA2-4DE5-95FF-3D43C4BC1A95}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e48749df-3746-4597-97ee-799f462add48"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9a67a83b-a5e1-4318-948d-450fbb0b26a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Feature/error during upload (#91) (#93)
Produce warning and error reports when uploading Budgets or Actuals from an Excel file.
Improve performance by reducing the numbers of read from the database and using a different way to read the Excel file.
Add heuristic message during the upload.
Lock the correct columns when downloading from the Edit Forecast page.
</commit_message>
<xml_diff>
--- a/forecast/test/test_assets/budget_upload_bad_data.xlsx
+++ b/forecast/test/test_assets/budget_upload_bad_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stronal/PycharmProjects/fido/forecast/test/test_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F78A10-DF02-5E46-9C81-42F37028E35C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9381B3F-FBA6-CC4A-80EC-6E6D3306E8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -934,7 +934,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1120,12 +1120,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1338,15 +1335,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADF255A-1CA2-4DE5-95FF-3D43C4BC1A95}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F34B647-70B2-425E-B00E-F8374E364F8C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e48749df-3746-4597-97ee-799f462add48"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9a67a83b-a5e1-4318-948d-450fbb0b26a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1371,18 +1380,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F34B647-70B2-425E-B00E-F8374E364F8C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADF255A-1CA2-4DE5-95FF-3D43C4BC1A95}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e48749df-3746-4597-97ee-799f462add48"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9a67a83b-a5e1-4318-948d-450fbb0b26a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>